<commit_message>
Update financial_file from dashboard
</commit_message>
<xml_diff>
--- a/data/financial_progress.xlsx
+++ b/data/financial_progress.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87805FF2-9B4F-F54A-BE7A-07D17B0932BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="5500" yWindow="4940" windowWidth="16100" windowHeight="13300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -103,8 +122,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,13 +186,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -211,7 +238,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -245,6 +272,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -279,9 +307,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -454,14 +483,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -495,7 +531,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -512,7 +548,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -520,7 +556,7 @@
         <v>408000000</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>408000000</v>
       </c>
       <c r="D4">
         <v>408000000</v>
@@ -529,7 +565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -546,7 +582,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -563,7 +599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -580,7 +616,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -597,7 +633,7 @@
         <v>25.36</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -614,7 +650,7 @@
         <v>20.83</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -631,7 +667,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -648,7 +684,7 @@
         <v>22.65</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -665,7 +701,7 @@
         <v>10.35</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -682,7 +718,7 @@
         <v>27.01</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -690,16 +726,16 @@
         <v>2571456305</v>
       </c>
       <c r="C14">
-        <v>1285728152.62</v>
+        <v>1285728152.6199999</v>
       </c>
       <c r="D14">
-        <v>1285728152.38</v>
+        <v>1285728152.3800001</v>
       </c>
       <c r="E14">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -713,10 +749,10 @@
         <v>258928312</v>
       </c>
       <c r="E15">
-        <v>87.06999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>87.07</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -733,7 +769,7 @@
         <v>31.36</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -747,10 +783,10 @@
         <v>106951200</v>
       </c>
       <c r="E17">
-        <v>77.09999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>77.099999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -758,16 +794,16 @@
         <v>12054156493</v>
       </c>
       <c r="C18">
-        <v>2186902526.534</v>
+        <v>2186902526.5339999</v>
       </c>
       <c r="D18">
-        <v>9867253966.466</v>
+        <v>9867253966.4659996</v>
       </c>
       <c r="E18">
         <v>18.14</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -784,7 +820,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -801,7 +837,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -809,16 +845,16 @@
         <v>12054156493</v>
       </c>
       <c r="C21">
-        <v>2186902526.534</v>
+        <v>2186902526.5339999</v>
       </c>
       <c r="D21">
-        <v>9867253966.466</v>
+        <v>9867253966.4659996</v>
       </c>
       <c r="E21">
         <v>18.14</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -835,7 +871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -852,7 +888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>

</xml_diff>